<commit_message>
filled out Test Case Document
</commit_message>
<xml_diff>
--- a/P2 RTM.xlsx
+++ b/P2 RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Chu\Desktop\P2\p2-bankberries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC7BC6E-F0AB-40F7-9D8A-92AE20114B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEBDFB9-24C1-42C0-BB2B-7854586D43C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D974DD7-2A15-4613-9C8A-1D5375C1A80D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7D974DD7-2A15-4613-9C8A-1D5375C1A80D}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="84">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -193,13 +193,168 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Test Writer</t>
+  </si>
+  <si>
+    <t>Test Review</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>User is on login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on main menu and
+view account details
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on main menu
+</t>
+  </si>
+  <si>
+    <t>User is on main menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on main menu and
+sees Apply for Loan
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on main menu 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on main menu can click
+checkings or savings
+</t>
+  </si>
+  <si>
+    <t>User clicks on either
+checking or savings
+and can see their individual</t>
+  </si>
+  <si>
+    <t>User can transer funds
+from checking to savings
+or vice versa</t>
+  </si>
+  <si>
+    <t>User types in their
+username and password,
+clicks Login</t>
+  </si>
+  <si>
+    <t>User types in wrong
+username and right password or,
+wrong password and right username,
+clicks Login</t>
+  </si>
+  <si>
+    <t>User logs in,
+user is on main menu,
+user clicks on either account to view details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User logs in,
+user is on main menu,
+user can click on links to be directed </t>
+  </si>
+  <si>
+    <t>User logs in and
+sees balances for either
+checking or savings</t>
+  </si>
+  <si>
+    <t>User logs in,
+clicks Apply for Loan,
+user fills out form,
+user clicks submit</t>
+  </si>
+  <si>
+    <t>User logs in,
+user can view their
+pending loan applications</t>
+  </si>
+  <si>
+    <t>User logs in,
+user is on main menu,
+user clicks either checking or savings,
+user can see indivdual balances</t>
+  </si>
+  <si>
+    <t>User logs in,
+user is on main menu,
+user clicks either checking or savings,
+user can trnsfer funds to another account
+user can see indivdual balances</t>
+  </si>
+  <si>
+    <t>User is on the main menu</t>
+  </si>
+  <si>
+    <t>An alert pops up and states,
+"Wrong username or password"</t>
+  </si>
+  <si>
+    <t>User can see button
+to click to view 
+account details</t>
+  </si>
+  <si>
+    <t>User can see link buttons and
+interact with them</t>
+  </si>
+  <si>
+    <t>User can see their
+chacking and savings
+funds</t>
+  </si>
+  <si>
+    <t>User successfully submited
+a filled out loan form</t>
+  </si>
+  <si>
+    <t>User can see their pending loan</t>
+  </si>
+  <si>
+    <t>User can see checkings balance or
+savings balance</t>
+  </si>
+  <si>
+    <t>User can see new balance of an account 
+they trnsfered funds to</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +388,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +413,13 @@
         <fgColor theme="7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -291,12 +457,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -310,8 +492,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -627,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CBE55-9AB7-41A9-80B0-F80F8F41E0AB}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,12 +1054,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737306D6-9266-4722-87D9-CF73D64D0081}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="6" max="6" width="24.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fixed testing and updated anchor id attributes
</commit_message>
<xml_diff>
--- a/P2 RTM.xlsx
+++ b/P2 RTM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Chu\Desktop\P2\p2-bankberries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\training-repos\p2-bankberries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4973D3-7826-44A0-B69E-A336F5344AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDEA5B2-B98F-4587-A530-EB3671405856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2115" yWindow="8145" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{7D974DD7-2A15-4613-9C8A-1D5375C1A80D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D974DD7-2A15-4613-9C8A-1D5375C1A80D}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Nicholas Chu</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>Test Case</t>
@@ -361,12 +358,18 @@
     <t xml:space="preserve">User clicks on savings account
 and can see details </t>
   </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,19 +396,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -422,12 +412,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -501,22 +491,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Accent4" xfId="1" builtinId="41"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -831,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CBE55-9AB7-41A9-80B0-F80F8F41E0AB}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,8 +884,8 @@
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>43</v>
+      <c r="F2" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -914,8 +904,8 @@
       <c r="E3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>43</v>
+      <c r="F3" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -934,8 +924,8 @@
       <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>43</v>
+      <c r="F4" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -943,19 +933,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>43</v>
+      <c r="F5" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -963,19 +953,19 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>43</v>
+      <c r="F6" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -994,8 +984,8 @@
       <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>43</v>
+      <c r="F7" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1014,8 +1004,8 @@
       <c r="E8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>43</v>
+      <c r="F8" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1034,8 +1024,8 @@
       <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
+      <c r="F9" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1054,13 +1044,13 @@
       <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>43</v>
+      <c r="F10" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -1074,8 +1064,8 @@
       <c r="E11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>43</v>
+      <c r="F11" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1088,265 +1078,292 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737306D6-9266-4722-87D9-CF73D64D0081}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="5"/>
-    <col min="6" max="6" width="24.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="24.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>54</v>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>56</v>
+      <c r="B7" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>